<commit_message>
Minor file reading changes
</commit_message>
<xml_diff>
--- a/Solution.xlsx
+++ b/Solution.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="353">
   <si>
     <t>Title</t>
   </si>
@@ -277,12 +277,6 @@
     <t>MONOPOLY</t>
   </si>
   <si>
-    <t>Игровой набор фигурки / игровой набор / набор для блейд-баттлов</t>
-  </si>
-  <si>
-    <t>Infinity Nado</t>
-  </si>
-  <si>
     <t>Rolly Polly / Бизиборд Бизидом со светом Смайлик, Развивающий домик</t>
   </si>
   <si>
@@ -763,24 +757,24 @@
     <t>Stickybook</t>
   </si>
   <si>
+    <t>Шахматы сувенирные Мария Стюарт, 45х45х10.3 см</t>
+  </si>
+  <si>
+    <t>All Souvenirs</t>
+  </si>
+  <si>
     <t>Шахматы сувенирные Древний Рим, 45х45х11 см</t>
   </si>
   <si>
     <t>Праздничный уют</t>
   </si>
   <si>
-    <t>Шахматы сувенирные Мария Стюарт, 45х45х10.3 см</t>
-  </si>
-  <si>
-    <t>All Souvenirs</t>
+    <t>Шахматы подарочные Римляне VS Галлы, 45х45х9.5 см</t>
   </si>
   <si>
     <t>Шахматы сувенирные Древний Египет, 45х45х9.5 см</t>
   </si>
   <si>
-    <t>Шахматы подарочные Римляне VS Галлы, 45х45х9.5 см</t>
-  </si>
-  <si>
     <t>Шахматы сувенирные Эль Сид, 38х38х8.3 см</t>
   </si>
   <si>
@@ -847,13 +841,13 @@
     <t>Настольная игра карточная</t>
   </si>
   <si>
+    <t>Набор из 4-х блистеров FORTNITE 2 2020</t>
+  </si>
+  <si>
+    <t>4 блистера наклеек FIFA 365-2022</t>
+  </si>
+  <si>
     <t>4 блистера наклеек Panini Три кота</t>
-  </si>
-  <si>
-    <t>4 блистера наклеек FIFA 365-2022</t>
-  </si>
-  <si>
-    <t>Набор из 4-х блистеров FORTNITE 2 2020</t>
   </si>
   <si>
     <t>Настольная игра Ежевички</t>
@@ -1460,7 +1454,7 @@
         <v>57266937</v>
       </c>
       <c r="D3">
-        <v>14142</v>
+        <v>14144</v>
       </c>
       <c r="E3">
         <v>1140</v>
@@ -1511,7 +1505,7 @@
         <v>71053760</v>
       </c>
       <c r="D6">
-        <v>3571</v>
+        <v>3573</v>
       </c>
       <c r="E6">
         <v>6000</v>
@@ -1545,7 +1539,7 @@
         <v>8694820</v>
       </c>
       <c r="D8">
-        <v>13206</v>
+        <v>13207</v>
       </c>
       <c r="E8">
         <v>4235</v>
@@ -1562,7 +1556,7 @@
         <v>56238068</v>
       </c>
       <c r="D9">
-        <v>14142</v>
+        <v>14144</v>
       </c>
       <c r="E9">
         <v>1620</v>
@@ -1579,7 +1573,7 @@
         <v>9960595</v>
       </c>
       <c r="D10">
-        <v>13206</v>
+        <v>13207</v>
       </c>
       <c r="E10">
         <v>4235</v>
@@ -1630,7 +1624,7 @@
         <v>8694821</v>
       </c>
       <c r="D13">
-        <v>13206</v>
+        <v>13207</v>
       </c>
       <c r="E13">
         <v>4235</v>
@@ -1647,7 +1641,7 @@
         <v>8694822</v>
       </c>
       <c r="D14">
-        <v>13206</v>
+        <v>13207</v>
       </c>
       <c r="E14">
         <v>4235</v>
@@ -1664,7 +1658,7 @@
         <v>51459547</v>
       </c>
       <c r="D15">
-        <v>4913</v>
+        <v>4914</v>
       </c>
       <c r="E15">
         <v>2450</v>
@@ -1698,7 +1692,7 @@
         <v>51459546</v>
       </c>
       <c r="D17">
-        <v>4913</v>
+        <v>4914</v>
       </c>
       <c r="E17">
         <v>2450</v>
@@ -1834,7 +1828,7 @@
         <v>51459548</v>
       </c>
       <c r="D25">
-        <v>4913</v>
+        <v>4914</v>
       </c>
       <c r="E25">
         <v>2450</v>
@@ -1885,7 +1879,7 @@
         <v>71053759</v>
       </c>
       <c r="D28">
-        <v>3571</v>
+        <v>3573</v>
       </c>
       <c r="E28">
         <v>4350</v>
@@ -1919,7 +1913,7 @@
         <v>38919468</v>
       </c>
       <c r="D30">
-        <v>1708</v>
+        <v>1710</v>
       </c>
       <c r="E30">
         <v>1850</v>
@@ -1936,7 +1930,7 @@
         <v>56238067</v>
       </c>
       <c r="D31">
-        <v>14142</v>
+        <v>14144</v>
       </c>
       <c r="E31">
         <v>1570</v>
@@ -2021,7 +2015,7 @@
         <v>2737172</v>
       </c>
       <c r="D36">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="E36">
         <v>1990</v>
@@ -2038,7 +2032,7 @@
         <v>31071277</v>
       </c>
       <c r="D37">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E37">
         <v>1331</v>
@@ -2276,7 +2270,7 @@
         <v>110781510</v>
       </c>
       <c r="D51">
-        <v>1406</v>
+        <v>1409</v>
       </c>
       <c r="E51">
         <v>3000</v>
@@ -2361,7 +2355,7 @@
         <v>71053752</v>
       </c>
       <c r="D56">
-        <v>3571</v>
+        <v>3573</v>
       </c>
       <c r="E56">
         <v>4350</v>
@@ -2389,33 +2383,33 @@
         <v>83</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="C58">
-        <v>10640325</v>
+        <v>78237462</v>
       </c>
       <c r="D58">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E58">
-        <v>4705</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" t="s">
         <v>85</v>
       </c>
-      <c r="B59" t="s">
-        <v>45</v>
-      </c>
       <c r="C59">
-        <v>78237462</v>
+        <v>57760226</v>
       </c>
       <c r="D59">
-        <v>77</v>
+        <v>925</v>
       </c>
       <c r="E59">
-        <v>3700</v>
+        <v>3625</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2426,13 +2420,13 @@
         <v>87</v>
       </c>
       <c r="C60">
-        <v>57760226</v>
+        <v>11966421</v>
       </c>
       <c r="D60">
-        <v>925</v>
+        <v>5861</v>
       </c>
       <c r="E60">
-        <v>3625</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2443,13 +2437,13 @@
         <v>89</v>
       </c>
       <c r="C61">
-        <v>11966421</v>
+        <v>33963390</v>
       </c>
       <c r="D61">
-        <v>5861</v>
+        <v>271</v>
       </c>
       <c r="E61">
-        <v>1491</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,13 +2454,13 @@
         <v>91</v>
       </c>
       <c r="C62">
-        <v>33963390</v>
+        <v>6448343</v>
       </c>
       <c r="D62">
-        <v>271</v>
+        <v>10621</v>
       </c>
       <c r="E62">
-        <v>2880</v>
+        <v>990</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,98 +2471,98 @@
         <v>93</v>
       </c>
       <c r="C63">
-        <v>6448343</v>
+        <v>60641694</v>
       </c>
       <c r="D63">
-        <v>10620</v>
+        <v>650</v>
       </c>
       <c r="E63">
-        <v>990</v>
+        <v>730</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>11</v>
+      </c>
+      <c r="B64" t="s">
         <v>94</v>
       </c>
-      <c r="B64" t="s">
-        <v>95</v>
-      </c>
       <c r="C64">
-        <v>60641694</v>
+        <v>30497938</v>
       </c>
       <c r="D64">
-        <v>648</v>
+        <v>351</v>
       </c>
       <c r="E64">
-        <v>730</v>
+        <v>7300</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
       <c r="B65" t="s">
         <v>96</v>
       </c>
       <c r="C65">
-        <v>30497938</v>
+        <v>3595159</v>
       </c>
       <c r="D65">
-        <v>351</v>
+        <v>3589</v>
       </c>
       <c r="E65">
-        <v>7300</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>98</v>
+        <v>79</v>
       </c>
       <c r="C66">
-        <v>3595159</v>
+        <v>40695769</v>
       </c>
       <c r="D66">
-        <v>3589</v>
+        <v>797</v>
       </c>
       <c r="E66">
-        <v>2761</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="C67">
-        <v>40695769</v>
+        <v>86853553</v>
       </c>
       <c r="D67">
-        <v>797</v>
+        <v>56</v>
       </c>
       <c r="E67">
-        <v>3500</v>
+        <v>6990</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>98</v>
       </c>
       <c r="C68">
-        <v>86853553</v>
+        <v>37879586</v>
       </c>
       <c r="D68">
-        <v>56</v>
+        <v>395</v>
       </c>
       <c r="E68">
-        <v>6990</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,13 +2573,13 @@
         <v>100</v>
       </c>
       <c r="C69">
-        <v>37879586</v>
+        <v>19911636</v>
       </c>
       <c r="D69">
-        <v>395</v>
+        <v>115</v>
       </c>
       <c r="E69">
-        <v>1182</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2596,13 +2590,13 @@
         <v>102</v>
       </c>
       <c r="C70">
-        <v>19911636</v>
+        <v>70408391</v>
       </c>
       <c r="D70">
-        <v>115</v>
+        <v>330</v>
       </c>
       <c r="E70">
-        <v>16500</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2610,13 +2604,13 @@
         <v>103</v>
       </c>
       <c r="B71" t="s">
-        <v>104</v>
+        <v>20</v>
       </c>
       <c r="C71">
-        <v>70408391</v>
+        <v>35256851</v>
       </c>
       <c r="D71">
-        <v>330</v>
+        <v>234</v>
       </c>
       <c r="E71">
         <v>5500</v>
@@ -2624,70 +2618,70 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" t="s">
         <v>105</v>
       </c>
-      <c r="B72" t="s">
-        <v>20</v>
-      </c>
       <c r="C72">
-        <v>35256851</v>
+        <v>4282599</v>
       </c>
       <c r="D72">
-        <v>234</v>
+        <v>1329</v>
       </c>
       <c r="E72">
-        <v>5500</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>106</v>
+        <v>31</v>
       </c>
       <c r="B73" t="s">
-        <v>107</v>
+        <v>26</v>
       </c>
       <c r="C73">
-        <v>4282599</v>
+        <v>47463479</v>
       </c>
       <c r="D73">
-        <v>1329</v>
+        <v>219</v>
       </c>
       <c r="E73">
-        <v>1878</v>
+        <v>3395</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B74" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C74">
-        <v>47463479</v>
+        <v>21308638</v>
       </c>
       <c r="D74">
-        <v>219</v>
+        <v>1517</v>
       </c>
       <c r="E74">
-        <v>3395</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="C75">
-        <v>21308638</v>
+        <v>13864309</v>
       </c>
       <c r="D75">
-        <v>1517</v>
+        <v>645</v>
       </c>
       <c r="E75">
-        <v>4812</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2698,13 +2692,13 @@
         <v>109</v>
       </c>
       <c r="C76">
-        <v>13864309</v>
+        <v>83744659</v>
       </c>
       <c r="D76">
-        <v>645</v>
+        <v>383</v>
       </c>
       <c r="E76">
-        <v>4469</v>
+        <v>5412</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2715,13 +2709,13 @@
         <v>111</v>
       </c>
       <c r="C77">
-        <v>83744659</v>
+        <v>69203891</v>
       </c>
       <c r="D77">
-        <v>383</v>
+        <v>81</v>
       </c>
       <c r="E77">
-        <v>5412</v>
+        <v>6100</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2732,13 +2726,13 @@
         <v>113</v>
       </c>
       <c r="C78">
-        <v>69203891</v>
+        <v>70564608</v>
       </c>
       <c r="D78">
-        <v>81</v>
+        <v>149</v>
       </c>
       <c r="E78">
-        <v>6100</v>
+        <v>7700</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2749,149 +2743,149 @@
         <v>115</v>
       </c>
       <c r="C79">
-        <v>70564608</v>
+        <v>45584098</v>
       </c>
       <c r="D79">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="E79">
-        <v>7700</v>
+        <v>2990</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>116</v>
+        <v>14</v>
       </c>
       <c r="B80" t="s">
-        <v>117</v>
+        <v>15</v>
       </c>
       <c r="C80">
-        <v>45584098</v>
+        <v>36795186</v>
       </c>
       <c r="D80">
-        <v>187</v>
+        <v>569</v>
       </c>
       <c r="E80">
-        <v>2990</v>
+        <v>2059</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="B81" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C81">
-        <v>36795186</v>
+        <v>18759140</v>
       </c>
       <c r="D81">
-        <v>569</v>
+        <v>2562</v>
       </c>
       <c r="E81">
-        <v>2059</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="C82">
-        <v>18759140</v>
+        <v>17783269</v>
       </c>
       <c r="D82">
-        <v>2562</v>
+        <v>106</v>
       </c>
       <c r="E82">
-        <v>1190</v>
+        <v>4699</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>38</v>
+      </c>
+      <c r="B83" t="s">
         <v>118</v>
       </c>
-      <c r="B83" t="s">
-        <v>119</v>
-      </c>
       <c r="C83">
-        <v>17783269</v>
+        <v>36168273</v>
       </c>
       <c r="D83">
-        <v>106</v>
+        <v>702</v>
       </c>
       <c r="E83">
-        <v>4699</v>
+        <v>2375</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>38</v>
+        <v>119</v>
       </c>
       <c r="B84" t="s">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="C84">
-        <v>36168273</v>
+        <v>57283976</v>
       </c>
       <c r="D84">
-        <v>702</v>
+        <v>544</v>
       </c>
       <c r="E84">
-        <v>2375</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>120</v>
+      </c>
+      <c r="B85" t="s">
         <v>121</v>
       </c>
-      <c r="B85" t="s">
-        <v>24</v>
-      </c>
       <c r="C85">
-        <v>57283976</v>
+        <v>32956363</v>
       </c>
       <c r="D85">
-        <v>544</v>
+        <v>1434</v>
       </c>
       <c r="E85">
-        <v>1083</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C86">
-        <v>32956363</v>
+        <v>70413077</v>
       </c>
       <c r="D86">
-        <v>1434</v>
+        <v>330</v>
       </c>
       <c r="E86">
-        <v>4544</v>
+        <v>3795</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="B87" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="C87">
-        <v>70413077</v>
+        <v>33756449</v>
       </c>
       <c r="D87">
-        <v>330</v>
+        <v>52</v>
       </c>
       <c r="E87">
-        <v>3795</v>
+        <v>17800</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2902,13 +2896,13 @@
         <v>125</v>
       </c>
       <c r="C88">
-        <v>33756449</v>
+        <v>10585894</v>
       </c>
       <c r="D88">
-        <v>52</v>
+        <v>497</v>
       </c>
       <c r="E88">
-        <v>17800</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2919,13 +2913,13 @@
         <v>127</v>
       </c>
       <c r="C89">
-        <v>10585894</v>
+        <v>26443731</v>
       </c>
       <c r="D89">
-        <v>497</v>
+        <v>84</v>
       </c>
       <c r="E89">
-        <v>1989</v>
+        <v>11259</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2936,13 +2930,13 @@
         <v>129</v>
       </c>
       <c r="C90">
-        <v>26443731</v>
+        <v>21277143</v>
       </c>
       <c r="D90">
-        <v>84</v>
+        <v>2395</v>
       </c>
       <c r="E90">
-        <v>11259</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2950,38 +2944,38 @@
         <v>130</v>
       </c>
       <c r="B91" t="s">
-        <v>131</v>
+        <v>59</v>
       </c>
       <c r="C91">
-        <v>21277143</v>
+        <v>21036203</v>
       </c>
       <c r="D91">
-        <v>2395</v>
+        <v>2756</v>
       </c>
       <c r="E91">
-        <v>1814</v>
+        <v>5342</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>132</v>
+        <v>38</v>
       </c>
       <c r="B92" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C92">
-        <v>21036203</v>
+        <v>37062208</v>
       </c>
       <c r="D92">
-        <v>2756</v>
+        <v>1025</v>
       </c>
       <c r="E92">
-        <v>5342</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B93" t="s">
         <v>68</v>
@@ -3007,7 +3001,7 @@
         <v>87704515</v>
       </c>
       <c r="D94">
-        <v>1406</v>
+        <v>1409</v>
       </c>
       <c r="E94">
         <v>300</v>
@@ -3015,10 +3009,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B95" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C95">
         <v>46710863</v>
@@ -3032,10 +3026,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B96" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C96">
         <v>66804281</v>
@@ -3049,10 +3043,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C97">
         <v>70799449</v>
@@ -3066,10 +3060,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B98" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C98">
         <v>63831677</v>
@@ -3083,7 +3077,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B99" t="s">
         <v>35</v>
@@ -3100,10 +3094,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B100" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C100">
         <v>17528816</v>
@@ -3117,10 +3111,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B101" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C101">
         <v>72787850</v>
@@ -3164,10 +3158,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2">
         <v>11561105</v>
@@ -3181,10 +3175,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C3">
         <v>72902996</v>
@@ -3198,10 +3192,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C4">
         <v>66372072</v>
@@ -3215,10 +3209,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5">
         <v>53900351</v>
@@ -3232,7 +3226,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -3266,10 +3260,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C8">
         <v>10533604</v>
@@ -3283,7 +3277,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
@@ -3309,7 +3303,7 @@
         <v>31071277</v>
       </c>
       <c r="D10">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="E10">
         <v>1331</v>
@@ -3317,10 +3311,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C11">
         <v>7531395</v>
@@ -3351,10 +3345,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C13">
         <v>10818997</v>
@@ -3368,10 +3362,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C14">
         <v>10898471</v>
@@ -3385,10 +3379,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C15">
         <v>86814248</v>
@@ -3402,10 +3396,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C16">
         <v>72274882</v>
@@ -3419,10 +3413,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C17">
         <v>61294300</v>
@@ -3436,10 +3430,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C18">
         <v>42505837</v>
@@ -3453,10 +3447,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C19">
         <v>86808488</v>
@@ -3470,10 +3464,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C20">
         <v>20873873</v>
@@ -3487,10 +3481,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C21">
         <v>72962110</v>
@@ -3504,10 +3498,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C22">
         <v>77482821</v>
@@ -3521,10 +3515,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C23">
         <v>37879586</v>
@@ -3538,10 +3532,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C24">
         <v>14612033</v>
@@ -3555,10 +3549,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C25">
         <v>45561429</v>
@@ -3581,7 +3575,7 @@
         <v>2737172</v>
       </c>
       <c r="D26">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="E26">
         <v>1990</v>
@@ -3589,10 +3583,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C27">
         <v>60711065</v>
@@ -3623,10 +3617,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C29">
         <v>70799350</v>
@@ -3640,10 +3634,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C30">
         <v>72060550</v>
@@ -3657,10 +3651,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C31">
         <v>33963390</v>
@@ -3674,10 +3668,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B32" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C32">
         <v>7531393</v>
@@ -3691,10 +3685,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B33" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C33">
         <v>2935299</v>
@@ -3708,10 +3702,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C34">
         <v>4426153</v>
@@ -3742,10 +3736,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C36">
         <v>4282599</v>
@@ -3759,10 +3753,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C37">
         <v>61982390</v>
@@ -3776,10 +3770,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C38">
         <v>77162239</v>
@@ -3793,10 +3787,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C39">
         <v>10818990</v>
@@ -3810,10 +3804,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C40">
         <v>70799449</v>
@@ -3827,10 +3821,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41">
         <v>17356605</v>
@@ -3844,10 +3838,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B42" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C42">
         <v>3235894</v>
@@ -3861,16 +3855,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C43">
         <v>4557086</v>
       </c>
       <c r="D43">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="E43">
         <v>761</v>
@@ -3878,10 +3872,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B44" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C44">
         <v>12025659</v>
@@ -3895,10 +3889,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B45" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C45">
         <v>59582132</v>
@@ -3912,10 +3906,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B46" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C46">
         <v>57684272</v>
@@ -3929,10 +3923,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B47" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C47">
         <v>56334321</v>
@@ -3946,10 +3940,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B48" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C48">
         <v>70463914</v>
@@ -3963,10 +3957,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C49">
         <v>16164286</v>
@@ -3997,10 +3991,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B51" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C51">
         <v>30181016</v>
@@ -4014,7 +4008,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B52" t="s">
         <v>68</v>
@@ -4031,10 +4025,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B53" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C53">
         <v>75783218</v>
@@ -4048,10 +4042,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C54">
         <v>8911720</v>
@@ -4065,10 +4059,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B55" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C55">
         <v>64620891</v>
@@ -4082,10 +4076,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B56" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C56">
         <v>18939543</v>
@@ -4099,10 +4093,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C57">
         <v>5567063</v>
@@ -4116,10 +4110,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C58">
         <v>56876012</v>
@@ -4133,10 +4127,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B59" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C59">
         <v>50122544</v>
@@ -4150,10 +4144,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B60" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C60">
         <v>5704050</v>
@@ -4167,10 +4161,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C61">
         <v>110871772</v>
@@ -4184,10 +4178,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B62" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C62">
         <v>37512009</v>
@@ -4201,10 +4195,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B63" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C63">
         <v>41286234</v>
@@ -4218,10 +4212,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B64" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C64">
         <v>48319244</v>
@@ -4235,7 +4229,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
@@ -4252,10 +4246,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C66">
         <v>12167132</v>
@@ -4269,10 +4263,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B67" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C67">
         <v>3048085</v>
@@ -4286,10 +4280,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B68" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C68">
         <v>73133928</v>
@@ -4303,10 +4297,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B69" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C69">
         <v>4715277</v>
@@ -4320,10 +4314,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B70" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C70">
         <v>44625721</v>
@@ -4337,10 +4331,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B71" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C71">
         <v>59371074</v>
@@ -4354,10 +4348,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B72" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C72">
         <v>65082328</v>
@@ -4371,10 +4365,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B73" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C73">
         <v>18995691</v>
@@ -4388,13 +4382,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B74" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C74">
-        <v>50946877</v>
+        <v>50946896</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -4405,13 +4399,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C75">
-        <v>50946896</v>
+        <v>50946877</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -4422,13 +4416,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B76" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C76">
-        <v>50946892</v>
+        <v>50946852</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -4439,13 +4433,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B77" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C77">
-        <v>50946852</v>
+        <v>50946892</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -4456,7 +4450,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B78" t="s">
         <v>246</v>
@@ -4473,10 +4467,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B79" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C79">
         <v>50946978</v>
@@ -4490,10 +4484,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B80" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C80">
         <v>115777117</v>
@@ -4507,10 +4501,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B81" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C81">
         <v>51089836</v>
@@ -4524,10 +4518,10 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B82" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C82">
         <v>50718646</v>
@@ -4541,10 +4535,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B83" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C83">
         <v>115870317</v>
@@ -4558,10 +4552,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B84" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C84">
         <v>51091239</v>
@@ -4575,10 +4569,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B85" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C85">
         <v>53901811</v>
@@ -4592,10 +4586,10 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B86" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C86">
         <v>53901810</v>
@@ -4609,10 +4603,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B87" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C87">
         <v>115673328</v>
@@ -4626,10 +4620,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B88" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C88">
         <v>59656720</v>
@@ -4643,10 +4637,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B89" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C89">
         <v>115777128</v>
@@ -4660,10 +4654,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B90" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C90">
         <v>95030142</v>
@@ -4677,10 +4671,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B91" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C91">
         <v>115664102</v>
@@ -4694,10 +4688,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B92" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C92">
         <v>116143163</v>
@@ -4711,10 +4705,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C93">
         <v>52305084</v>
@@ -4728,13 +4722,13 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B94" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C94">
-        <v>95030140</v>
+        <v>95030143</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -4745,7 +4739,7 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C95">
         <v>95030161</v>
@@ -4759,13 +4753,13 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B96" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C96">
-        <v>95030143</v>
+        <v>95030140</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -4776,10 +4770,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B97" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C97">
         <v>64888212</v>
@@ -4793,10 +4787,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B98" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C98">
         <v>115873367</v>
@@ -4810,10 +4804,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B99" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C99">
         <v>61165091</v>
@@ -4827,10 +4821,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B100" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C100">
         <v>66104037</v>
@@ -4844,10 +4838,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B101" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C101">
         <v>115924307</v>
@@ -4891,10 +4885,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C2">
         <v>66070237</v>
@@ -4908,10 +4902,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C3">
         <v>27379808</v>
@@ -4925,16 +4919,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C4">
         <v>13615125</v>
       </c>
       <c r="D4">
-        <v>4898</v>
+        <v>4899</v>
       </c>
       <c r="E4">
         <v>8990</v>
@@ -4942,16 +4936,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C5">
         <v>22903474</v>
       </c>
       <c r="D5">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E5">
         <v>28990</v>
@@ -4959,10 +4953,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B6" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C6">
         <v>66070236</v>
@@ -4976,10 +4970,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C7">
         <v>67866097</v>
@@ -4993,10 +4987,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B8" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C8">
         <v>84018675</v>
@@ -5010,10 +5004,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C9">
         <v>51728993</v>
@@ -5027,16 +5021,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C10">
         <v>44587792</v>
       </c>
       <c r="D10">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="E10">
         <v>29990</v>
@@ -5044,10 +5038,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C11">
         <v>111244822</v>
@@ -5061,16 +5055,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B12" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C12">
         <v>84018137</v>
       </c>
       <c r="D12">
-        <v>4898</v>
+        <v>4899</v>
       </c>
       <c r="E12">
         <v>8990</v>
@@ -5078,10 +5072,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C13">
         <v>66069789</v>
@@ -5095,16 +5089,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C14">
         <v>88962425</v>
       </c>
       <c r="D14">
-        <v>4898</v>
+        <v>4899</v>
       </c>
       <c r="E14">
         <v>8990</v>
@@ -5112,10 +5106,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C15">
         <v>51728992</v>
@@ -5129,10 +5123,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B16" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C16">
         <v>39766970</v>
@@ -5146,10 +5140,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B17" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C17">
         <v>43105060</v>
@@ -5163,10 +5157,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C18">
         <v>110523995</v>
@@ -5180,10 +5174,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C19">
         <v>67866096</v>
@@ -5197,16 +5191,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B20" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C20">
         <v>27379809</v>
       </c>
       <c r="D20">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E20">
         <v>26499</v>
@@ -5214,10 +5208,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B21" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C21">
         <v>28199303</v>
@@ -5231,10 +5225,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C22">
         <v>78487259</v>
@@ -5248,10 +5242,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B23" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C23">
         <v>86123936</v>
@@ -5265,10 +5259,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B24" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C24">
         <v>28980742</v>
@@ -5282,10 +5276,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B25" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C25">
         <v>44950987</v>
@@ -5299,10 +5293,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C26">
         <v>72288318</v>
@@ -5316,10 +5310,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C27">
         <v>72295496</v>
@@ -5333,10 +5327,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B28" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C28">
         <v>28199302</v>
@@ -5350,10 +5344,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C29">
         <v>53399132</v>
@@ -5367,10 +5361,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B30" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C30">
         <v>35683124</v>
@@ -5384,10 +5378,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B31" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C31">
         <v>67866095</v>
@@ -5401,10 +5395,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B32" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C32">
         <v>72295495</v>
@@ -5418,10 +5412,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C33">
         <v>46015369</v>
@@ -5435,10 +5429,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C34">
         <v>66069790</v>
@@ -5452,10 +5446,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B35" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C35">
         <v>113254271</v>
@@ -5469,10 +5463,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B36" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C36">
         <v>46015370</v>
@@ -5486,10 +5480,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C37">
         <v>50424584</v>
@@ -5503,10 +5497,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C38">
         <v>39769257</v>
@@ -5520,10 +5514,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B39" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C39">
         <v>114713906</v>
@@ -5537,10 +5531,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B40" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C40">
         <v>39769256</v>
@@ -5554,10 +5548,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B41" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C41">
         <v>45997083</v>
@@ -5571,10 +5565,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B42" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C42">
         <v>51728991</v>
@@ -5588,10 +5582,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B43" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C43">
         <v>111244812</v>
@@ -5605,10 +5599,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B44" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C44">
         <v>73027267</v>
@@ -5622,10 +5616,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B45" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C45">
         <v>30967922</v>
@@ -5639,10 +5633,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C46">
         <v>111864727</v>
@@ -5656,10 +5650,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B47" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C47">
         <v>67983222</v>
@@ -5673,10 +5667,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B48" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C48">
         <v>60418878</v>
@@ -5690,10 +5684,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B49" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C49">
         <v>67865980</v>
@@ -5707,10 +5701,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B50" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C50">
         <v>111864728</v>
@@ -5724,10 +5718,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B51" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C51">
         <v>114316934</v>
@@ -5741,10 +5735,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B52" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C52">
         <v>80640174</v>
@@ -5758,10 +5752,10 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B53" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C53">
         <v>51730036</v>
@@ -5775,10 +5769,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B54" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C54">
         <v>65373048</v>
@@ -5792,10 +5786,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B55" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C55">
         <v>45997084</v>
@@ -5809,10 +5803,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B56" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C56">
         <v>30967920</v>
@@ -5826,10 +5820,10 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B57" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C57">
         <v>84888191</v>
@@ -5843,10 +5837,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B58" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C58">
         <v>72288320</v>
@@ -5860,10 +5854,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B59" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C59">
         <v>48077005</v>
@@ -5877,10 +5871,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B60" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C60">
         <v>26830014</v>
@@ -5894,10 +5888,10 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B61" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C61">
         <v>114713905</v>
@@ -5911,10 +5905,10 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B62" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C62">
         <v>43105061</v>
@@ -5928,10 +5922,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B63" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C63">
         <v>110521531</v>
@@ -5945,10 +5939,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B64" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C64">
         <v>47716114</v>
@@ -5962,10 +5956,10 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B65" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C65">
         <v>113254274</v>
@@ -5979,10 +5973,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B66" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C66">
         <v>30967930</v>
@@ -5996,10 +5990,10 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B67" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C67">
         <v>113254270</v>
@@ -6013,10 +6007,10 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B68" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C68">
         <v>61914203</v>
@@ -6030,10 +6024,10 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B69" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C69">
         <v>60418879</v>
@@ -6047,10 +6041,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B70" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C70">
         <v>113244919</v>
@@ -6064,10 +6058,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B71" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C71">
         <v>90680712</v>
@@ -6081,16 +6075,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B72" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C72">
         <v>55919141</v>
       </c>
       <c r="D72">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E72">
         <v>18990</v>
@@ -6098,10 +6092,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B73" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C73">
         <v>91052042</v>
@@ -6115,10 +6109,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B74" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C74">
         <v>111864107</v>
@@ -6132,10 +6126,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B75" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C75">
         <v>36873567</v>
@@ -6149,10 +6143,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B76" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C76">
         <v>44583543</v>
@@ -6166,10 +6160,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B77" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C77">
         <v>55917992</v>
@@ -6183,10 +6177,10 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B78" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C78">
         <v>75664919</v>
@@ -6200,10 +6194,10 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B79" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C79">
         <v>61900894</v>
@@ -6217,10 +6211,10 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B80" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C80">
         <v>91604390</v>
@@ -6234,10 +6228,10 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B81" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C81">
         <v>91604388</v>
@@ -6251,10 +6245,10 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B82" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C82">
         <v>63884383</v>
@@ -6268,10 +6262,10 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B83" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C83">
         <v>111864106</v>
@@ -6285,10 +6279,10 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B84" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C84">
         <v>113254248</v>
@@ -6302,10 +6296,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B85" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C85">
         <v>43819444</v>
@@ -6319,10 +6313,10 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B86" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C86">
         <v>46595796</v>
@@ -6336,10 +6330,10 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B87" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C87">
         <v>113254269</v>
@@ -6353,10 +6347,10 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B88" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C88">
         <v>75665278</v>
@@ -6370,10 +6364,10 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B89" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C89">
         <v>40654195</v>
@@ -6387,10 +6381,10 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B90" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C90">
         <v>113254234</v>
@@ -6404,10 +6398,10 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B91" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C91">
         <v>62556357</v>
@@ -6421,10 +6415,10 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B92" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C92">
         <v>113254231</v>
@@ -6438,10 +6432,10 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B93" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C93">
         <v>24717029</v>
@@ -6455,10 +6449,10 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B94" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C94">
         <v>114447592</v>
@@ -6472,10 +6466,10 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B95" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C95">
         <v>36877787</v>
@@ -6489,10 +6483,10 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B96" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C96">
         <v>63753745</v>
@@ -6506,10 +6500,10 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B97" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C97">
         <v>67865979</v>
@@ -6523,10 +6517,10 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B98" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C98">
         <v>44584205</v>
@@ -6540,10 +6534,10 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B99" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C99">
         <v>61900895</v>
@@ -6557,10 +6551,10 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B100" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C100">
         <v>88966809</v>
@@ -6574,10 +6568,10 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B101" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C101">
         <v>110520088</v>

</xml_diff>